<commit_message>
more new excel files
</commit_message>
<xml_diff>
--- a/HuskyTAC/Test.xlsx
+++ b/HuskyTAC/Test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="382">
   <si>
     <t>Equipment Number</t>
   </si>
@@ -650,6 +650,18 @@
     <t>CHI1232918-CHI8403963</t>
   </si>
   <si>
+    <t>TLLU4616515</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>7032045328</t>
+  </si>
+  <si>
+    <t>ONEYHKGV78076404</t>
+  </si>
+  <si>
     <t>SEGU1390068</t>
   </si>
   <si>
@@ -1022,6 +1034,15 @@
     <t>DJPDXA4162486</t>
   </si>
   <si>
+    <t>BEAU2750146</t>
+  </si>
+  <si>
+    <t>7032045325</t>
+  </si>
+  <si>
+    <t>ONEYTPEV26277500</t>
+  </si>
+  <si>
     <t>TRLU9731277</t>
   </si>
   <si>
@@ -1116,9 +1137,6 @@
   </si>
   <si>
     <t>TCLU3519929</t>
-  </si>
-  <si>
-    <t>01</t>
   </si>
   <si>
     <t>7032045315</t>
@@ -1184,7 +1202,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2445,13 +2463,13 @@
         <v>212</v>
       </c>
       <c r="B69" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>112</v>
+        <v>213</v>
       </c>
       <c r="D69" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E69" t="s">
         <v>214</v>
@@ -2465,10 +2483,10 @@
         <v>216</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="C70" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="D70" t="s">
         <v>217</v>
@@ -2485,10 +2503,10 @@
         <v>220</v>
       </c>
       <c r="B71" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="D71" t="s">
         <v>221</v>
@@ -2525,10 +2543,10 @@
         <v>228</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="C73" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="D73" t="s">
         <v>229</v>
@@ -2545,33 +2563,33 @@
         <v>232</v>
       </c>
       <c r="B74" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="C74" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" t="s">
         <v>233</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>234</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
         <v>235</v>
-      </c>
-      <c r="F74" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>236</v>
+      </c>
+      <c r="B75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C75" t="s">
         <v>237</v>
       </c>
-      <c r="B75" t="s">
-        <v>87</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>238</v>
-      </c>
-      <c r="D75" t="s">
-        <v>239</v>
       </c>
       <c r="E75" t="s">
         <v>239</v>
@@ -2585,40 +2603,42 @@
         <v>241</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C76" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="D76" t="s">
-        <v>242</v>
-      </c>
-      <c r="E76"/>
+        <v>243</v>
+      </c>
+      <c r="E76" t="s">
+        <v>243</v>
+      </c>
       <c r="F76" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C77" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="D77" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E77"/>
       <c r="F77" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
@@ -2627,31 +2647,29 @@
         <v>12</v>
       </c>
       <c r="D78" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E78"/>
       <c r="F78" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B79" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="D79" t="s">
+        <v>252</v>
+      </c>
+      <c r="E79"/>
+      <c r="F79" t="s">
         <v>250</v>
-      </c>
-      <c r="E79" t="s">
-        <v>251</v>
-      </c>
-      <c r="F79" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="80">
@@ -2668,15 +2686,15 @@
         <v>254</v>
       </c>
       <c r="E80" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F80" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B81" t="s">
         <v>87</v>
@@ -2685,18 +2703,18 @@
         <v>112</v>
       </c>
       <c r="D81" t="s">
+        <v>258</v>
+      </c>
+      <c r="E81" t="s">
+        <v>255</v>
+      </c>
+      <c r="F81" t="s">
         <v>256</v>
-      </c>
-      <c r="E81" t="s">
-        <v>251</v>
-      </c>
-      <c r="F81" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B82" t="s">
         <v>87</v>
@@ -2705,18 +2723,18 @@
         <v>112</v>
       </c>
       <c r="D82" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E82" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F82" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B83" t="s">
         <v>87</v>
@@ -2725,49 +2743,49 @@
         <v>112</v>
       </c>
       <c r="D83" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E83" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F83" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B84" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C84" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D84" t="s">
-        <v>262</v>
-      </c>
-      <c r="E84"/>
+        <v>264</v>
+      </c>
+      <c r="E84" t="s">
+        <v>255</v>
+      </c>
       <c r="F84" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C85" t="s">
-        <v>31</v>
+        <v>117</v>
       </c>
       <c r="D85" t="s">
-        <v>265</v>
-      </c>
-      <c r="E85" t="s">
         <v>266</v>
       </c>
+      <c r="E85"/>
       <c r="F85" t="s">
         <v>267</v>
       </c>
@@ -2780,39 +2798,39 @@
         <v>7</v>
       </c>
       <c r="C86" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D86" t="s">
         <v>269</v>
       </c>
-      <c r="E86"/>
+      <c r="E86" t="s">
+        <v>270</v>
+      </c>
       <c r="F86" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B87" t="s">
         <v>7</v>
       </c>
       <c r="C87" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D87" t="s">
-        <v>272</v>
-      </c>
-      <c r="E87" t="s">
-        <v>272</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="E87"/>
       <c r="F87" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
@@ -2821,33 +2839,33 @@
         <v>31</v>
       </c>
       <c r="D88" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E88" t="s">
-        <v>230</v>
+        <v>276</v>
       </c>
       <c r="F88" t="s">
-        <v>231</v>
+        <v>277</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>277</v>
+        <v>31</v>
       </c>
       <c r="D89" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E89" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
       <c r="F89" t="s">
-        <v>279</v>
+        <v>235</v>
       </c>
     </row>
     <row r="90">
@@ -2858,99 +2876,101 @@
         <v>7</v>
       </c>
       <c r="C90" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D90" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E90" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="F90" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>284</v>
+      </c>
+      <c r="B91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" t="s">
         <v>281</v>
       </c>
-      <c r="B91" t="s">
-        <v>7</v>
-      </c>
-      <c r="C91" t="s">
-        <v>277</v>
-      </c>
       <c r="D91" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E91" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="F91" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>285</v>
+      </c>
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>281</v>
+      </c>
+      <c r="D92" t="s">
         <v>282</v>
       </c>
-      <c r="B92" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" t="s">
-        <v>277</v>
-      </c>
-      <c r="D92" t="s">
-        <v>278</v>
-      </c>
       <c r="E92" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="F92" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>286</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>281</v>
+      </c>
+      <c r="D93" t="s">
+        <v>282</v>
+      </c>
+      <c r="E93" t="s">
+        <v>282</v>
+      </c>
+      <c r="F93" t="s">
         <v>283</v>
-      </c>
-      <c r="B93" t="s">
-        <v>7</v>
-      </c>
-      <c r="C93" t="s">
-        <v>277</v>
-      </c>
-      <c r="D93" t="s">
-        <v>278</v>
-      </c>
-      <c r="E93" t="s">
-        <v>278</v>
-      </c>
-      <c r="F93" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B94" t="s">
         <v>7</v>
       </c>
       <c r="C94" t="s">
-        <v>12</v>
+        <v>281</v>
       </c>
       <c r="D94" t="s">
-        <v>285</v>
-      </c>
-      <c r="E94"/>
+        <v>282</v>
+      </c>
+      <c r="E94" t="s">
+        <v>282</v>
+      </c>
       <c r="F94" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B95" t="s">
         <v>7</v>
@@ -2959,16 +2979,16 @@
         <v>12</v>
       </c>
       <c r="D95" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E95"/>
       <c r="F95" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B96" t="s">
         <v>7</v>
@@ -2977,143 +2997,141 @@
         <v>12</v>
       </c>
       <c r="D96" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E96"/>
       <c r="F96" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B97" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C97" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="D97" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E97"/>
       <c r="F97" t="s">
-        <v>292</v>
+        <v>250</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B98" t="s">
         <v>87</v>
       </c>
       <c r="C98" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="D98" t="s">
-        <v>294</v>
-      </c>
-      <c r="E98" t="s">
-        <v>251</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="E98"/>
       <c r="F98" t="s">
-        <v>252</v>
+        <v>296</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B99" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="C99" t="s">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="D99" t="s">
-        <v>296</v>
-      </c>
-      <c r="E99"/>
+        <v>298</v>
+      </c>
+      <c r="E99" t="s">
+        <v>255</v>
+      </c>
       <c r="F99" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B100" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C100" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="D100" t="s">
-        <v>298</v>
-      </c>
-      <c r="E100" t="s">
-        <v>298</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E100"/>
       <c r="F100" t="s">
-        <v>299</v>
+        <v>250</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B101" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="C101" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="D101" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E101" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F101" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B102" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C102" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="D102" t="s">
-        <v>304</v>
-      </c>
-      <c r="E102"/>
+        <v>305</v>
+      </c>
+      <c r="E102" t="s">
+        <v>305</v>
+      </c>
       <c r="F102" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B103" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C103" t="s">
-        <v>233</v>
+        <v>88</v>
       </c>
       <c r="D103" t="s">
-        <v>307</v>
-      </c>
-      <c r="E103" t="s">
         <v>308</v>
       </c>
+      <c r="E103"/>
       <c r="F103" t="s">
         <v>309</v>
       </c>
@@ -3123,22 +3141,24 @@
         <v>310</v>
       </c>
       <c r="B104" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="C104" t="s">
-        <v>88</v>
+        <v>237</v>
       </c>
       <c r="D104" t="s">
         <v>311</v>
       </c>
-      <c r="E104"/>
+      <c r="E104" t="s">
+        <v>312</v>
+      </c>
       <c r="F104" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B105" t="s">
         <v>87</v>
@@ -3147,16 +3167,16 @@
         <v>88</v>
       </c>
       <c r="D105" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E105"/>
       <c r="F105" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B106" t="s">
         <v>87</v>
@@ -3165,16 +3185,16 @@
         <v>88</v>
       </c>
       <c r="D106" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E106"/>
       <c r="F106" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B107" t="s">
         <v>87</v>
@@ -3183,31 +3203,29 @@
         <v>88</v>
       </c>
       <c r="D107" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E107"/>
       <c r="F107" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B108" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C108" t="s">
-        <v>233</v>
+        <v>88</v>
       </c>
       <c r="D108" t="s">
-        <v>321</v>
-      </c>
-      <c r="E108" t="s">
-        <v>322</v>
-      </c>
+        <v>323</v>
+      </c>
+      <c r="E108"/>
       <c r="F108" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="109">
@@ -3215,10 +3233,10 @@
         <v>324</v>
       </c>
       <c r="B109" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="C109" t="s">
-        <v>112</v>
+        <v>237</v>
       </c>
       <c r="D109" t="s">
         <v>325</v>
@@ -3238,19 +3256,21 @@
         <v>87</v>
       </c>
       <c r="C110" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="D110" t="s">
         <v>329</v>
       </c>
-      <c r="E110"/>
+      <c r="E110" t="s">
+        <v>330</v>
+      </c>
       <c r="F110" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B111" t="s">
         <v>87</v>
@@ -3259,51 +3279,49 @@
         <v>88</v>
       </c>
       <c r="D111" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E111"/>
       <c r="F111" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B112" t="s">
         <v>87</v>
       </c>
       <c r="C112" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="D112" t="s">
-        <v>335</v>
-      </c>
-      <c r="E112" t="s">
-        <v>251</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="E112"/>
       <c r="F112" t="s">
-        <v>252</v>
+        <v>337</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B113" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C113" t="s">
-        <v>233</v>
+        <v>112</v>
       </c>
       <c r="D113" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E113" t="s">
-        <v>338</v>
+        <v>255</v>
       </c>
       <c r="F113" t="s">
-        <v>339</v>
+        <v>256</v>
       </c>
     </row>
     <row r="114">
@@ -3311,138 +3329,140 @@
         <v>340</v>
       </c>
       <c r="B114" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s">
+        <v>213</v>
+      </c>
+      <c r="D114" t="s">
         <v>341</v>
       </c>
-      <c r="C114" t="s">
+      <c r="E114" t="s">
+        <v>341</v>
+      </c>
+      <c r="F114" t="s">
         <v>342</v>
-      </c>
-      <c r="D114" t="s">
-        <v>343</v>
-      </c>
-      <c r="E114" t="s">
-        <v>343</v>
-      </c>
-      <c r="F114" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B115" t="s">
         <v>39</v>
       </c>
       <c r="C115" t="s">
-        <v>117</v>
+        <v>237</v>
       </c>
       <c r="D115" t="s">
+        <v>344</v>
+      </c>
+      <c r="E115" t="s">
+        <v>345</v>
+      </c>
+      <c r="F115" t="s">
         <v>346</v>
-      </c>
-      <c r="E115"/>
-      <c r="F115" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
+        <v>347</v>
+      </c>
+      <c r="B116" t="s">
         <v>348</v>
       </c>
-      <c r="B116" t="s">
-        <v>7</v>
-      </c>
       <c r="C116" t="s">
-        <v>31</v>
+        <v>349</v>
       </c>
       <c r="D116" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E116" t="s">
-        <v>230</v>
+        <v>350</v>
       </c>
       <c r="F116" t="s">
-        <v>231</v>
+        <v>351</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B117" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="C117" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D117" t="s">
-        <v>351</v>
-      </c>
-      <c r="E117" t="s">
-        <v>352</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="E117"/>
       <c r="F117" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B118" t="s">
         <v>7</v>
       </c>
       <c r="C118" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D118" t="s">
-        <v>355</v>
-      </c>
-      <c r="E118"/>
+        <v>356</v>
+      </c>
+      <c r="E118" t="s">
+        <v>234</v>
+      </c>
       <c r="F118" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B119" t="s">
         <v>87</v>
       </c>
       <c r="C119" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="D119" t="s">
-        <v>357</v>
-      </c>
-      <c r="E119"/>
+        <v>358</v>
+      </c>
+      <c r="E119" t="s">
+        <v>359</v>
+      </c>
       <c r="F119" t="s">
-        <v>317</v>
+        <v>360</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B120" t="s">
         <v>7</v>
       </c>
       <c r="C120" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D120" t="s">
-        <v>359</v>
-      </c>
-      <c r="E120" t="s">
-        <v>360</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="E120"/>
       <c r="F120" t="s">
-        <v>361</v>
+        <v>250</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B121" t="s">
         <v>87</v>
@@ -3451,11 +3471,11 @@
         <v>88</v>
       </c>
       <c r="D121" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E121"/>
       <c r="F121" t="s">
-        <v>364</v>
+        <v>321</v>
       </c>
     </row>
     <row r="122">
@@ -3463,57 +3483,57 @@
         <v>365</v>
       </c>
       <c r="B122" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="C122" t="s">
-        <v>233</v>
+        <v>31</v>
       </c>
       <c r="D122" t="s">
         <v>366</v>
       </c>
       <c r="E122" t="s">
-        <v>322</v>
+        <v>367</v>
       </c>
       <c r="F122" t="s">
-        <v>323</v>
+        <v>368</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B123" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="C123" t="s">
-        <v>368</v>
+        <v>88</v>
       </c>
       <c r="D123" t="s">
-        <v>369</v>
-      </c>
-      <c r="E123" t="s">
-        <v>369</v>
-      </c>
+        <v>370</v>
+      </c>
+      <c r="E123"/>
       <c r="F123" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B124" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C124" t="s">
-        <v>12</v>
+        <v>237</v>
       </c>
       <c r="D124" t="s">
-        <v>372</v>
-      </c>
-      <c r="E124"/>
+        <v>373</v>
+      </c>
+      <c r="E124" t="s">
+        <v>326</v>
+      </c>
       <c r="F124" t="s">
-        <v>373</v>
+        <v>327</v>
       </c>
     </row>
     <row r="125">
@@ -3524,14 +3544,52 @@
         <v>7</v>
       </c>
       <c r="C125" t="s">
-        <v>12</v>
+        <v>213</v>
       </c>
       <c r="D125" t="s">
         <v>375</v>
       </c>
-      <c r="E125"/>
+      <c r="E125" t="s">
+        <v>375</v>
+      </c>
       <c r="F125" t="s">
-        <v>246</v>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>377</v>
+      </c>
+      <c r="B126" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" t="s">
+        <v>12</v>
+      </c>
+      <c r="D126" t="s">
+        <v>378</v>
+      </c>
+      <c r="E126"/>
+      <c r="F126" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>380</v>
+      </c>
+      <c r="B127" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" t="s">
+        <v>12</v>
+      </c>
+      <c r="D127" t="s">
+        <v>381</v>
+      </c>
+      <c r="E127"/>
+      <c r="F127" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>